<commit_message>
se estima el error fault al publicar
</commit_message>
<xml_diff>
--- a/publish/ProjectsToPublish.xlsx
+++ b/publish/ProjectsToPublish.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Jenkins\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Jenkins\publish\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B9E90C1-9051-4738-8F8D-585A02F98792}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89F7BFEB-0F6A-4763-90C4-E301A3B33AA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{232C2E75-DCBC-4924-AE5A-0A313BE6BAAE}"/>
   </bookViews>
@@ -34,22 +34,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Projects</t>
   </si>
   <si>
-    <t>TestRuben</t>
-  </si>
-  <si>
-    <t>TestRuben1</t>
+    <t>AmxCoFijPosPromo023_B26</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -65,16 +62,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -82,14 +91,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFD1D1D1"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFD1D1D1"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFD1D1D1"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFD1D1D1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -405,10 +432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA1EBC66-685E-42AD-85C6-222DFBBC3ADD}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -422,14 +449,18 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
+      <c r="A3" s="2"/>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>